<commit_message>
add model activity and some APIs
</commit_message>
<xml_diff>
--- a/document/gpe_model.xlsx
+++ b/document/gpe_model.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="10320" yWindow="440" windowWidth="26360" windowHeight="14920" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="960" yWindow="440" windowWidth="26360" windowHeight="14920" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="dictionary" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="145">
   <si>
     <t>name</t>
   </si>
@@ -424,6 +424,45 @@
   </si>
   <si>
     <t>List&lt;Message&gt;</t>
+  </si>
+  <si>
+    <t>/del</t>
+  </si>
+  <si>
+    <t>void</t>
+  </si>
+  <si>
+    <t>/act</t>
+  </si>
+  <si>
+    <t>List&lt;Activity&gt;</t>
+  </si>
+  <si>
+    <t>/detail</t>
+  </si>
+  <si>
+    <t>Activity</t>
+  </si>
+  <si>
+    <t>/csnews</t>
+  </si>
+  <si>
+    <t>List&lt;Cnews&gt;</t>
+  </si>
+  <si>
+    <t>/update</t>
+  </si>
+  <si>
+    <t>/all</t>
+  </si>
+  <si>
+    <t>List&lt;User&gt;</t>
+  </si>
+  <si>
+    <t>/sh</t>
+  </si>
+  <si>
+    <t>test</t>
   </si>
 </sst>
 </file>
@@ -461,7 +500,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -477,6 +516,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -556,7 +601,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -589,7 +634,10 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -616,10 +664,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -930,7 +987,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="14" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -941,7 +998,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="14"/>
+      <c r="A3" s="15"/>
       <c r="B3" s="5" t="s">
         <v>0</v>
       </c>
@@ -953,7 +1010,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="14"/>
+      <c r="A4" s="15"/>
       <c r="B4" s="5" t="s">
         <v>1</v>
       </c>
@@ -962,7 +1019,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="14"/>
+      <c r="A5" s="15"/>
       <c r="B5" s="5" t="s">
         <v>2</v>
       </c>
@@ -971,7 +1028,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="14"/>
+      <c r="A6" s="15"/>
       <c r="B6" s="5" t="s">
         <v>3</v>
       </c>
@@ -983,7 +1040,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="14"/>
+      <c r="A7" s="15"/>
       <c r="B7" s="5" t="s">
         <v>81</v>
       </c>
@@ -992,7 +1049,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="14"/>
+      <c r="A8" s="15"/>
       <c r="B8" s="5" t="s">
         <v>40</v>
       </c>
@@ -1001,7 +1058,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="14"/>
+      <c r="A9" s="15"/>
       <c r="B9" s="5" t="s">
         <v>21</v>
       </c>
@@ -1010,7 +1067,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="15"/>
+      <c r="A10" s="16"/>
       <c r="B10" s="5" t="s">
         <v>52</v>
       </c>
@@ -1019,7 +1076,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="14" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="5" t="s">
@@ -1030,7 +1087,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="14"/>
+      <c r="A12" s="15"/>
       <c r="B12" s="5" t="s">
         <v>5</v>
       </c>
@@ -1039,7 +1096,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="14"/>
+      <c r="A13" s="15"/>
       <c r="B13" s="5" t="s">
         <v>7</v>
       </c>
@@ -1051,7 +1108,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="14"/>
+      <c r="A14" s="15"/>
       <c r="B14" s="5" t="s">
         <v>8</v>
       </c>
@@ -1060,7 +1117,7 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="14"/>
+      <c r="A15" s="15"/>
       <c r="B15" s="5" t="s">
         <v>9</v>
       </c>
@@ -1069,7 +1126,7 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="15"/>
+      <c r="A16" s="16"/>
       <c r="B16" s="5" t="s">
         <v>82</v>
       </c>
@@ -1081,7 +1138,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="13" t="s">
+      <c r="A17" s="14" t="s">
         <v>16</v>
       </c>
       <c r="B17" s="5" t="s">
@@ -1092,7 +1149,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="14"/>
+      <c r="A18" s="15"/>
       <c r="B18" s="5" t="s">
         <v>11</v>
       </c>
@@ -1101,7 +1158,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="14"/>
+      <c r="A19" s="15"/>
       <c r="B19" s="5" t="s">
         <v>12</v>
       </c>
@@ -1113,7 +1170,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="14"/>
+      <c r="A20" s="15"/>
       <c r="B20" s="5" t="s">
         <v>13</v>
       </c>
@@ -1122,7 +1179,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="14"/>
+      <c r="A21" s="15"/>
       <c r="B21" s="5" t="s">
         <v>14</v>
       </c>
@@ -1134,7 +1191,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="14"/>
+      <c r="A22" s="15"/>
       <c r="B22" s="5" t="s">
         <v>9</v>
       </c>
@@ -1143,7 +1200,7 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="14"/>
+      <c r="A23" s="15"/>
       <c r="B23" s="5" t="s">
         <v>15</v>
       </c>
@@ -1152,7 +1209,7 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="14"/>
+      <c r="A24" s="15"/>
       <c r="B24" s="5" t="s">
         <v>83</v>
       </c>
@@ -1164,7 +1221,7 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="14"/>
+      <c r="A25" s="15"/>
       <c r="B25" s="5" t="s">
         <v>84</v>
       </c>
@@ -1176,7 +1233,7 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="14"/>
+      <c r="A26" s="15"/>
       <c r="B26" s="5" t="s">
         <v>0</v>
       </c>
@@ -1185,7 +1242,7 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="14"/>
+      <c r="A27" s="15"/>
       <c r="B27" s="5" t="s">
         <v>48</v>
       </c>
@@ -1194,7 +1251,7 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="15"/>
+      <c r="A28" s="16"/>
       <c r="B28" s="5" t="s">
         <v>71</v>
       </c>
@@ -1203,7 +1260,7 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="13" t="s">
+      <c r="A29" s="14" t="s">
         <v>17</v>
       </c>
       <c r="B29" s="5" t="s">
@@ -1214,7 +1271,7 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="14"/>
+      <c r="A30" s="15"/>
       <c r="B30" s="5" t="s">
         <v>0</v>
       </c>
@@ -1226,7 +1283,7 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="14"/>
+      <c r="A31" s="15"/>
       <c r="B31" s="5" t="s">
         <v>18</v>
       </c>
@@ -1235,7 +1292,7 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="14"/>
+      <c r="A32" s="15"/>
       <c r="B32" s="5" t="s">
         <v>19</v>
       </c>
@@ -1247,7 +1304,7 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="14"/>
+      <c r="A33" s="15"/>
       <c r="B33" s="5" t="s">
         <v>20</v>
       </c>
@@ -1256,7 +1313,7 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" s="15"/>
+      <c r="A34" s="16"/>
       <c r="B34" s="5" t="s">
         <v>21</v>
       </c>
@@ -1265,7 +1322,7 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="13" t="s">
+      <c r="A35" s="14" t="s">
         <v>22</v>
       </c>
       <c r="B35" s="5" t="s">
@@ -1276,7 +1333,7 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="14"/>
+      <c r="A36" s="15"/>
       <c r="B36" s="5" t="s">
         <v>0</v>
       </c>
@@ -1288,7 +1345,7 @@
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="15"/>
+      <c r="A37" s="16"/>
       <c r="B37" s="5" t="s">
         <v>21</v>
       </c>
@@ -1297,7 +1354,7 @@
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="13" t="s">
+      <c r="A38" s="14" t="s">
         <v>24</v>
       </c>
       <c r="B38" s="5" t="s">
@@ -1308,7 +1365,7 @@
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" s="14"/>
+      <c r="A39" s="15"/>
       <c r="B39" s="5" t="s">
         <v>82</v>
       </c>
@@ -1320,7 +1377,7 @@
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40" s="14"/>
+      <c r="A40" s="15"/>
       <c r="B40" s="5" t="s">
         <v>7</v>
       </c>
@@ -1332,7 +1389,7 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" s="15"/>
+      <c r="A41" s="16"/>
       <c r="B41" s="5" t="s">
         <v>25</v>
       </c>
@@ -1341,7 +1398,7 @@
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" s="13" t="s">
+      <c r="A42" s="14" t="s">
         <v>26</v>
       </c>
       <c r="B42" s="5" t="s">
@@ -1350,42 +1407,42 @@
       <c r="C42" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="D42" s="19" t="s">
+      <c r="D42" s="20" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" s="14"/>
+      <c r="A43" s="15"/>
       <c r="B43" s="5" t="s">
         <v>28</v>
       </c>
       <c r="C43" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="D43" s="19"/>
+      <c r="D43" s="20"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" s="14"/>
+      <c r="A44" s="15"/>
       <c r="B44" s="5" t="s">
         <v>29</v>
       </c>
       <c r="C44" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="D44" s="19"/>
+      <c r="D44" s="20"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="15"/>
+      <c r="A45" s="16"/>
       <c r="B45" s="5" t="s">
         <v>30</v>
       </c>
       <c r="C45" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="D45" s="19"/>
+      <c r="D45" s="20"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" s="13" t="s">
+      <c r="A46" s="14" t="s">
         <v>31</v>
       </c>
       <c r="B46" s="5" t="s">
@@ -1396,7 +1453,7 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47" s="14"/>
+      <c r="A47" s="15"/>
       <c r="B47" s="5" t="s">
         <v>32</v>
       </c>
@@ -1408,7 +1465,7 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A48" s="15"/>
+      <c r="A48" s="16"/>
       <c r="B48" s="5" t="s">
         <v>25</v>
       </c>
@@ -1417,7 +1474,7 @@
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" s="13" t="s">
+      <c r="A49" s="14" t="s">
         <v>33</v>
       </c>
       <c r="B49" s="5" t="s">
@@ -1428,7 +1485,7 @@
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50" s="14"/>
+      <c r="A50" s="15"/>
       <c r="B50" s="5" t="s">
         <v>34</v>
       </c>
@@ -1437,7 +1494,7 @@
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51" s="14"/>
+      <c r="A51" s="15"/>
       <c r="B51" s="5" t="s">
         <v>35</v>
       </c>
@@ -1449,7 +1506,7 @@
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A52" s="15"/>
+      <c r="A52" s="16"/>
       <c r="B52" s="5" t="s">
         <v>36</v>
       </c>
@@ -1461,7 +1518,7 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A53" s="16" t="s">
+      <c r="A53" s="17" t="s">
         <v>37</v>
       </c>
       <c r="B53" s="10" t="s">
@@ -1472,7 +1529,7 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A54" s="17"/>
+      <c r="A54" s="18"/>
       <c r="B54" s="10" t="s">
         <v>38</v>
       </c>
@@ -1481,7 +1538,7 @@
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A55" s="17"/>
+      <c r="A55" s="18"/>
       <c r="B55" s="10" t="s">
         <v>39</v>
       </c>
@@ -1490,7 +1547,7 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56" s="18"/>
+      <c r="A56" s="19"/>
       <c r="B56" s="10" t="s">
         <v>40</v>
       </c>
@@ -1499,7 +1556,7 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A57" s="13" t="s">
+      <c r="A57" s="14" t="s">
         <v>6</v>
       </c>
       <c r="B57" s="5" t="s">
@@ -1510,7 +1567,7 @@
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A58" s="14"/>
+      <c r="A58" s="15"/>
       <c r="B58" s="5" t="s">
         <v>0</v>
       </c>
@@ -1522,7 +1579,7 @@
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59" s="14"/>
+      <c r="A59" s="15"/>
       <c r="B59" s="5" t="s">
         <v>41</v>
       </c>
@@ -1531,7 +1588,7 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A60" s="15"/>
+      <c r="A60" s="16"/>
       <c r="B60" s="5" t="s">
         <v>21</v>
       </c>
@@ -1540,7 +1597,7 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A61" s="13" t="s">
+      <c r="A61" s="14" t="s">
         <v>42</v>
       </c>
       <c r="B61" s="5" t="s">
@@ -1551,7 +1608,7 @@
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A62" s="14"/>
+      <c r="A62" s="15"/>
       <c r="B62" s="5" t="s">
         <v>0</v>
       </c>
@@ -1563,7 +1620,7 @@
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A63" s="15"/>
+      <c r="A63" s="16"/>
       <c r="B63" s="5" t="s">
         <v>21</v>
       </c>
@@ -1572,7 +1629,7 @@
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A64" s="20" t="s">
+      <c r="A64" s="21" t="s">
         <v>43</v>
       </c>
       <c r="B64" s="5" t="s">
@@ -1583,7 +1640,7 @@
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A65" s="20"/>
+      <c r="A65" s="21"/>
       <c r="B65" s="5" t="s">
         <v>0</v>
       </c>
@@ -1592,7 +1649,7 @@
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A66" s="20"/>
+      <c r="A66" s="21"/>
       <c r="B66" s="5" t="s">
         <v>2</v>
       </c>
@@ -1601,7 +1658,7 @@
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A67" s="20"/>
+      <c r="A67" s="21"/>
       <c r="B67" s="5" t="s">
         <v>9</v>
       </c>
@@ -1610,7 +1667,7 @@
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A68" s="20"/>
+      <c r="A68" s="21"/>
       <c r="B68" s="5" t="s">
         <v>3</v>
       </c>
@@ -1619,7 +1676,7 @@
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A69" s="20"/>
+      <c r="A69" s="21"/>
       <c r="B69" s="5" t="s">
         <v>1</v>
       </c>
@@ -1628,7 +1685,7 @@
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A70" s="20"/>
+      <c r="A70" s="21"/>
       <c r="B70" s="5" t="s">
         <v>85</v>
       </c>
@@ -1640,7 +1697,7 @@
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A71" s="20"/>
+      <c r="A71" s="21"/>
       <c r="B71" s="5" t="s">
         <v>21</v>
       </c>
@@ -1649,7 +1706,7 @@
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A72" s="20"/>
+      <c r="A72" s="21"/>
       <c r="B72" s="5" t="s">
         <v>15</v>
       </c>
@@ -1658,7 +1715,7 @@
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A73" s="20"/>
+      <c r="A73" s="21"/>
       <c r="B73" s="5" t="s">
         <v>81</v>
       </c>
@@ -1670,7 +1727,7 @@
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A74" s="20"/>
+      <c r="A74" s="21"/>
       <c r="B74" s="5" t="s">
         <v>82</v>
       </c>
@@ -1682,7 +1739,7 @@
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A75" s="20"/>
+      <c r="A75" s="21"/>
       <c r="B75" s="5" t="s">
         <v>64</v>
       </c>
@@ -1691,7 +1748,7 @@
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A76" s="20"/>
+      <c r="A76" s="21"/>
       <c r="B76" s="5" t="s">
         <v>65</v>
       </c>
@@ -1700,7 +1757,7 @@
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A77" s="20"/>
+      <c r="A77" s="21"/>
       <c r="B77" s="5" t="s">
         <v>66</v>
       </c>
@@ -1709,7 +1766,7 @@
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A78" s="13" t="s">
+      <c r="A78" s="14" t="s">
         <v>47</v>
       </c>
       <c r="B78" s="7" t="s">
@@ -1720,7 +1777,7 @@
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A79" s="14"/>
+      <c r="A79" s="15"/>
       <c r="B79" s="7" t="s">
         <v>49</v>
       </c>
@@ -1729,7 +1786,7 @@
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A80" s="14"/>
+      <c r="A80" s="15"/>
       <c r="B80" s="7" t="s">
         <v>50</v>
       </c>
@@ -1738,7 +1795,7 @@
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A81" s="14"/>
+      <c r="A81" s="15"/>
       <c r="B81" s="7" t="s">
         <v>86</v>
       </c>
@@ -1747,7 +1804,7 @@
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A82" s="14"/>
+      <c r="A82" s="15"/>
       <c r="B82" s="7" t="s">
         <v>87</v>
       </c>
@@ -1756,7 +1813,7 @@
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A83" s="14"/>
+      <c r="A83" s="15"/>
       <c r="B83" s="7" t="s">
         <v>74</v>
       </c>
@@ -1765,7 +1822,7 @@
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A84" s="14"/>
+      <c r="A84" s="15"/>
       <c r="B84" s="7" t="s">
         <v>75</v>
       </c>
@@ -1774,7 +1831,7 @@
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A85" s="14"/>
+      <c r="A85" s="15"/>
       <c r="B85" s="7" t="s">
         <v>76</v>
       </c>
@@ -1783,7 +1840,7 @@
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A86" s="14"/>
+      <c r="A86" s="15"/>
       <c r="B86" s="7" t="s">
         <v>77</v>
       </c>
@@ -1792,7 +1849,7 @@
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A87" s="14"/>
+      <c r="A87" s="15"/>
       <c r="B87" s="7" t="s">
         <v>72</v>
       </c>
@@ -1801,7 +1858,7 @@
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A88" s="13" t="s">
+      <c r="A88" s="14" t="s">
         <v>70</v>
       </c>
       <c r="B88" s="5" t="s">
@@ -1812,7 +1869,7 @@
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A89" s="14"/>
+      <c r="A89" s="15"/>
       <c r="B89" s="8" t="s">
         <v>72</v>
       </c>
@@ -1821,7 +1878,7 @@
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A90" s="13" t="s">
+      <c r="A90" s="14" t="s">
         <v>78</v>
       </c>
       <c r="B90" s="5" t="s">
@@ -1832,7 +1889,7 @@
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A91" s="14"/>
+      <c r="A91" s="15"/>
       <c r="B91" s="5" t="s">
         <v>51</v>
       </c>
@@ -1841,7 +1898,7 @@
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A92" s="15"/>
+      <c r="A92" s="16"/>
       <c r="B92" s="5" t="s">
         <v>72</v>
       </c>
@@ -1875,17 +1932,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="3"/>
     <col min="2" max="2" width="14.33203125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="22"/>
+    <col min="3" max="3" width="10.83203125" style="13"/>
     <col min="4" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
@@ -1896,7 +1953,7 @@
       <c r="B1" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="12" t="s">
         <v>108</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -1919,7 +1976,7 @@
       <c r="B2" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="20"/>
+      <c r="C2" s="14"/>
       <c r="D2" s="5" t="s">
         <v>109</v>
       </c>
@@ -1934,7 +1991,7 @@
       <c r="B3" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="C3" s="20"/>
+      <c r="C3" s="15"/>
       <c r="D3" s="5" t="s">
         <v>110</v>
       </c>
@@ -1949,7 +2006,7 @@
       <c r="B4" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="C4" s="20"/>
+      <c r="C4" s="15"/>
       <c r="D4" s="5" t="s">
         <v>117</v>
       </c>
@@ -1966,11 +2023,13 @@
       <c r="B5" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="C5" s="20"/>
+      <c r="C5" s="15"/>
       <c r="D5" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="E5" s="5"/>
+      <c r="E5" s="5" t="s">
+        <v>41</v>
+      </c>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
     </row>
@@ -1981,14 +2040,16 @@
       <c r="B6" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="C6" s="20"/>
+      <c r="C6" s="15"/>
       <c r="D6" s="5" t="s">
         <v>120</v>
       </c>
       <c r="E6" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F6" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="F6" s="5"/>
       <c r="G6" s="5"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -1998,14 +2059,16 @@
       <c r="B7" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="C7" s="20"/>
+      <c r="C7" s="15"/>
       <c r="D7" s="5" t="s">
         <v>111</v>
       </c>
       <c r="E7" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F7" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="F7" s="5"/>
       <c r="G7" s="5"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -2015,14 +2078,16 @@
       <c r="B8" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="C8" s="20"/>
+      <c r="C8" s="15"/>
       <c r="D8" s="5" t="s">
         <v>112</v>
       </c>
       <c r="E8" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F8" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="F8" s="5"/>
       <c r="G8" s="5"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -2030,31 +2095,33 @@
         <v>92</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="C9" s="20"/>
-      <c r="D9" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="E9" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="C9" s="15"/>
+      <c r="D9" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="F9" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
+      <c r="G9" s="7"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>92</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="C10" s="20"/>
+        <v>98</v>
+      </c>
+      <c r="C10" s="15"/>
       <c r="D10" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>80</v>
+        <v>41</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>88</v>
@@ -2063,128 +2130,130 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" s="20" t="s">
-        <v>107</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="C11" s="16"/>
       <c r="D11" s="5" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G11" s="5"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" s="20"/>
-      <c r="D12" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="G12" s="5"/>
+      <c r="A12" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="C12" s="24" t="s">
+        <v>134</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="G12" s="7"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" s="20"/>
-      <c r="D13" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="G13" s="5"/>
+      <c r="A13" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="C13" s="25"/>
+      <c r="D13" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="G13" s="7"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" s="20"/>
-      <c r="D14" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="G14" s="5"/>
+      <c r="A14" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="C14" s="26"/>
+      <c r="D14" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="20"/>
+      <c r="C15" s="14" t="s">
+        <v>107</v>
+      </c>
       <c r="D15" s="5" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="F15" s="5"/>
+        <v>89</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>90</v>
+      </c>
       <c r="G15" s="5"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="20"/>
+      <c r="C16" s="15"/>
       <c r="D16" s="5" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="F16" s="5"/>
+        <v>89</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>90</v>
+      </c>
       <c r="G16" s="5"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
         <v>91</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="12" t="s">
-        <v>115</v>
-      </c>
+      <c r="C17" s="15"/>
       <c r="D17" s="5" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>89</v>
@@ -2194,93 +2263,322 @@
       </c>
       <c r="G17" s="5"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>91</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C18" s="13" t="s">
-        <v>122</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="C18" s="15"/>
       <c r="D18" s="5" t="s">
-        <v>123</v>
+        <v>103</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>125</v>
+        <v>89</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+        <v>90</v>
+      </c>
+      <c r="G18" s="5"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
         <v>92</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="C19" s="14"/>
+        <v>16</v>
+      </c>
+      <c r="C19" s="15"/>
       <c r="D19" s="5" t="s">
-        <v>126</v>
+        <v>104</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>88</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="F19" s="5"/>
       <c r="G19" s="5"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
         <v>92</v>
       </c>
       <c r="B20" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" s="15"/>
+      <c r="D20" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" s="16"/>
+      <c r="D21" s="23" t="s">
+        <v>140</v>
+      </c>
+      <c r="E21" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="F21" s="23"/>
+      <c r="G21" s="23"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23" s="15"/>
+      <c r="D23" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C24" s="16"/>
+      <c r="D24" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="G24" s="5"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B26" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="C20" s="14"/>
-      <c r="D20" s="5" t="s">
+      <c r="C26" s="15"/>
+      <c r="D26" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="G26" s="5"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="C27" s="15"/>
+      <c r="D27" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="E20" s="5" t="s">
+      <c r="E27" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="F20" s="5" t="s">
+      <c r="F27" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="G20" s="5"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="5" t="s">
+      <c r="G27" s="5"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B28" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C21" s="15"/>
-      <c r="D21" s="5" t="s">
+      <c r="C28" s="15"/>
+      <c r="D28" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="E21" s="5" t="s">
+      <c r="E28" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="F21" s="5" t="s">
+      <c r="F28" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="G21" s="5" t="s">
+      <c r="G28" s="5" t="s">
         <v>129</v>
       </c>
     </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="C29" s="15"/>
+      <c r="D29" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="C30" s="15"/>
+      <c r="D30" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7"/>
+      <c r="H30" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C31" s="16"/>
+      <c r="D31" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="F31" s="7"/>
+      <c r="G31" s="7"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="C32" s="14" t="s">
+        <v>143</v>
+      </c>
+      <c r="D32" s="23" t="s">
+        <v>105</v>
+      </c>
+      <c r="E32" s="23"/>
+      <c r="F32" s="23"/>
+      <c r="G32" s="23"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C33" s="15"/>
+      <c r="D33" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="E33" s="23"/>
+      <c r="F33" s="23"/>
+      <c r="G33" s="23"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C34" s="16"/>
+      <c r="D34" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="E34" s="23"/>
+      <c r="F34" s="23"/>
+      <c r="G34" s="23"/>
+    </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="C11:C16"/>
-    <mergeCell ref="C2:C10"/>
-    <mergeCell ref="C18:C21"/>
+  <mergeCells count="6">
+    <mergeCell ref="C2:C11"/>
+    <mergeCell ref="C32:C34"/>
+    <mergeCell ref="C25:C31"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="C15:C21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
fixed model with @JsonManagedReference and @JsonBackReference annotation
</commit_message>
<xml_diff>
--- a/document/gpe_model.xlsx
+++ b/document/gpe_model.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="161">
   <si>
     <t>name</t>
   </si>
@@ -429,9 +429,6 @@
     <t>/del</t>
   </si>
   <si>
-    <t>void</t>
-  </si>
-  <si>
     <t>/act</t>
   </si>
   <si>
@@ -463,6 +460,57 @@
   </si>
   <si>
     <t>test</t>
+  </si>
+  <si>
+    <t>/post</t>
+  </si>
+  <si>
+    <t>activity</t>
+  </si>
+  <si>
+    <t>Cnews</t>
+  </si>
+  <si>
+    <t>/mng</t>
+  </si>
+  <si>
+    <t>/adcns</t>
+  </si>
+  <si>
+    <t>/advns</t>
+  </si>
+  <si>
+    <t>/adns</t>
+  </si>
+  <si>
+    <t>/aduf</t>
+  </si>
+  <si>
+    <t>fol</t>
+  </si>
+  <si>
+    <t>/aduj</t>
+  </si>
+  <si>
+    <t>/deuj</t>
+  </si>
+  <si>
+    <t>club</t>
+  </si>
+  <si>
+    <t>/dluf</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>/activity</t>
+  </si>
+  <si>
+    <t>/cdetail</t>
+  </si>
+  <si>
+    <t>/vdetail</t>
   </si>
 </sst>
 </file>
@@ -500,7 +548,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -522,6 +570,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -601,7 +655,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -640,6 +694,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -664,20 +721,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -960,7 +1008,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D92"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
@@ -987,7 +1035,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="15" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -998,7 +1046,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="15"/>
+      <c r="A3" s="16"/>
       <c r="B3" s="5" t="s">
         <v>0</v>
       </c>
@@ -1010,7 +1058,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="15"/>
+      <c r="A4" s="16"/>
       <c r="B4" s="5" t="s">
         <v>1</v>
       </c>
@@ -1019,7 +1067,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="15"/>
+      <c r="A5" s="16"/>
       <c r="B5" s="5" t="s">
         <v>2</v>
       </c>
@@ -1028,7 +1076,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="15"/>
+      <c r="A6" s="16"/>
       <c r="B6" s="5" t="s">
         <v>3</v>
       </c>
@@ -1040,7 +1088,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="15"/>
+      <c r="A7" s="16"/>
       <c r="B7" s="5" t="s">
         <v>81</v>
       </c>
@@ -1049,7 +1097,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="15"/>
+      <c r="A8" s="16"/>
       <c r="B8" s="5" t="s">
         <v>40</v>
       </c>
@@ -1058,7 +1106,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="15"/>
+      <c r="A9" s="16"/>
       <c r="B9" s="5" t="s">
         <v>21</v>
       </c>
@@ -1067,7 +1115,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="16"/>
+      <c r="A10" s="17"/>
       <c r="B10" s="5" t="s">
         <v>52</v>
       </c>
@@ -1076,7 +1124,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="15" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="5" t="s">
@@ -1087,7 +1135,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="15"/>
+      <c r="A12" s="16"/>
       <c r="B12" s="5" t="s">
         <v>5</v>
       </c>
@@ -1096,7 +1144,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="15"/>
+      <c r="A13" s="16"/>
       <c r="B13" s="5" t="s">
         <v>7</v>
       </c>
@@ -1108,7 +1156,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="15"/>
+      <c r="A14" s="16"/>
       <c r="B14" s="5" t="s">
         <v>8</v>
       </c>
@@ -1117,7 +1165,7 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="15"/>
+      <c r="A15" s="16"/>
       <c r="B15" s="5" t="s">
         <v>9</v>
       </c>
@@ -1126,7 +1174,7 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="16"/>
+      <c r="A16" s="17"/>
       <c r="B16" s="5" t="s">
         <v>82</v>
       </c>
@@ -1138,7 +1186,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="14" t="s">
+      <c r="A17" s="15" t="s">
         <v>16</v>
       </c>
       <c r="B17" s="5" t="s">
@@ -1149,7 +1197,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="15"/>
+      <c r="A18" s="16"/>
       <c r="B18" s="5" t="s">
         <v>11</v>
       </c>
@@ -1158,7 +1206,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="15"/>
+      <c r="A19" s="16"/>
       <c r="B19" s="5" t="s">
         <v>12</v>
       </c>
@@ -1170,7 +1218,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="15"/>
+      <c r="A20" s="16"/>
       <c r="B20" s="5" t="s">
         <v>13</v>
       </c>
@@ -1179,7 +1227,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="15"/>
+      <c r="A21" s="16"/>
       <c r="B21" s="5" t="s">
         <v>14</v>
       </c>
@@ -1191,7 +1239,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="15"/>
+      <c r="A22" s="16"/>
       <c r="B22" s="5" t="s">
         <v>9</v>
       </c>
@@ -1200,7 +1248,7 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="15"/>
+      <c r="A23" s="16"/>
       <c r="B23" s="5" t="s">
         <v>15</v>
       </c>
@@ -1209,7 +1257,7 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="15"/>
+      <c r="A24" s="16"/>
       <c r="B24" s="5" t="s">
         <v>83</v>
       </c>
@@ -1221,7 +1269,7 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="15"/>
+      <c r="A25" s="16"/>
       <c r="B25" s="5" t="s">
         <v>84</v>
       </c>
@@ -1233,7 +1281,7 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="15"/>
+      <c r="A26" s="16"/>
       <c r="B26" s="5" t="s">
         <v>0</v>
       </c>
@@ -1242,7 +1290,7 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="15"/>
+      <c r="A27" s="16"/>
       <c r="B27" s="5" t="s">
         <v>48</v>
       </c>
@@ -1251,7 +1299,7 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="16"/>
+      <c r="A28" s="17"/>
       <c r="B28" s="5" t="s">
         <v>71</v>
       </c>
@@ -1260,7 +1308,7 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="14" t="s">
+      <c r="A29" s="15" t="s">
         <v>17</v>
       </c>
       <c r="B29" s="5" t="s">
@@ -1271,7 +1319,7 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="15"/>
+      <c r="A30" s="16"/>
       <c r="B30" s="5" t="s">
         <v>0</v>
       </c>
@@ -1283,7 +1331,7 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="15"/>
+      <c r="A31" s="16"/>
       <c r="B31" s="5" t="s">
         <v>18</v>
       </c>
@@ -1292,7 +1340,7 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="15"/>
+      <c r="A32" s="16"/>
       <c r="B32" s="5" t="s">
         <v>19</v>
       </c>
@@ -1304,7 +1352,7 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="15"/>
+      <c r="A33" s="16"/>
       <c r="B33" s="5" t="s">
         <v>20</v>
       </c>
@@ -1313,7 +1361,7 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" s="16"/>
+      <c r="A34" s="17"/>
       <c r="B34" s="5" t="s">
         <v>21</v>
       </c>
@@ -1322,7 +1370,7 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="14" t="s">
+      <c r="A35" s="15" t="s">
         <v>22</v>
       </c>
       <c r="B35" s="5" t="s">
@@ -1333,7 +1381,7 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="15"/>
+      <c r="A36" s="16"/>
       <c r="B36" s="5" t="s">
         <v>0</v>
       </c>
@@ -1345,7 +1393,7 @@
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="16"/>
+      <c r="A37" s="17"/>
       <c r="B37" s="5" t="s">
         <v>21</v>
       </c>
@@ -1354,7 +1402,7 @@
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="14" t="s">
+      <c r="A38" s="15" t="s">
         <v>24</v>
       </c>
       <c r="B38" s="5" t="s">
@@ -1365,7 +1413,7 @@
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" s="15"/>
+      <c r="A39" s="16"/>
       <c r="B39" s="5" t="s">
         <v>82</v>
       </c>
@@ -1377,7 +1425,7 @@
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40" s="15"/>
+      <c r="A40" s="16"/>
       <c r="B40" s="5" t="s">
         <v>7</v>
       </c>
@@ -1389,7 +1437,7 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" s="16"/>
+      <c r="A41" s="17"/>
       <c r="B41" s="5" t="s">
         <v>25</v>
       </c>
@@ -1398,7 +1446,7 @@
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" s="14" t="s">
+      <c r="A42" s="15" t="s">
         <v>26</v>
       </c>
       <c r="B42" s="5" t="s">
@@ -1407,42 +1455,42 @@
       <c r="C42" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="D42" s="20" t="s">
+      <c r="D42" s="21" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" s="15"/>
+      <c r="A43" s="16"/>
       <c r="B43" s="5" t="s">
         <v>28</v>
       </c>
       <c r="C43" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="D43" s="20"/>
+      <c r="D43" s="21"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" s="15"/>
+      <c r="A44" s="16"/>
       <c r="B44" s="5" t="s">
         <v>29</v>
       </c>
       <c r="C44" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="D44" s="20"/>
+      <c r="D44" s="21"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="16"/>
+      <c r="A45" s="17"/>
       <c r="B45" s="5" t="s">
         <v>30</v>
       </c>
       <c r="C45" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="D45" s="20"/>
+      <c r="D45" s="21"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" s="14" t="s">
+      <c r="A46" s="15" t="s">
         <v>31</v>
       </c>
       <c r="B46" s="5" t="s">
@@ -1453,7 +1501,7 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47" s="15"/>
+      <c r="A47" s="16"/>
       <c r="B47" s="5" t="s">
         <v>32</v>
       </c>
@@ -1465,7 +1513,7 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A48" s="16"/>
+      <c r="A48" s="17"/>
       <c r="B48" s="5" t="s">
         <v>25</v>
       </c>
@@ -1474,7 +1522,7 @@
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" s="14" t="s">
+      <c r="A49" s="15" t="s">
         <v>33</v>
       </c>
       <c r="B49" s="5" t="s">
@@ -1485,7 +1533,7 @@
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50" s="15"/>
+      <c r="A50" s="16"/>
       <c r="B50" s="5" t="s">
         <v>34</v>
       </c>
@@ -1494,7 +1542,7 @@
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51" s="15"/>
+      <c r="A51" s="16"/>
       <c r="B51" s="5" t="s">
         <v>35</v>
       </c>
@@ -1506,7 +1554,7 @@
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A52" s="16"/>
+      <c r="A52" s="17"/>
       <c r="B52" s="5" t="s">
         <v>36</v>
       </c>
@@ -1518,7 +1566,7 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A53" s="17" t="s">
+      <c r="A53" s="18" t="s">
         <v>37</v>
       </c>
       <c r="B53" s="10" t="s">
@@ -1529,7 +1577,7 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A54" s="18"/>
+      <c r="A54" s="19"/>
       <c r="B54" s="10" t="s">
         <v>38</v>
       </c>
@@ -1538,7 +1586,7 @@
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A55" s="18"/>
+      <c r="A55" s="19"/>
       <c r="B55" s="10" t="s">
         <v>39</v>
       </c>
@@ -1547,7 +1595,7 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56" s="19"/>
+      <c r="A56" s="20"/>
       <c r="B56" s="10" t="s">
         <v>40</v>
       </c>
@@ -1556,7 +1604,7 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A57" s="14" t="s">
+      <c r="A57" s="15" t="s">
         <v>6</v>
       </c>
       <c r="B57" s="5" t="s">
@@ -1567,7 +1615,7 @@
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A58" s="15"/>
+      <c r="A58" s="16"/>
       <c r="B58" s="5" t="s">
         <v>0</v>
       </c>
@@ -1579,7 +1627,7 @@
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59" s="15"/>
+      <c r="A59" s="16"/>
       <c r="B59" s="5" t="s">
         <v>41</v>
       </c>
@@ -1588,7 +1636,7 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A60" s="16"/>
+      <c r="A60" s="17"/>
       <c r="B60" s="5" t="s">
         <v>21</v>
       </c>
@@ -1597,7 +1645,7 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A61" s="14" t="s">
+      <c r="A61" s="15" t="s">
         <v>42</v>
       </c>
       <c r="B61" s="5" t="s">
@@ -1608,7 +1656,7 @@
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A62" s="15"/>
+      <c r="A62" s="16"/>
       <c r="B62" s="5" t="s">
         <v>0</v>
       </c>
@@ -1620,7 +1668,7 @@
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A63" s="16"/>
+      <c r="A63" s="17"/>
       <c r="B63" s="5" t="s">
         <v>21</v>
       </c>
@@ -1629,7 +1677,7 @@
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A64" s="21" t="s">
+      <c r="A64" s="22" t="s">
         <v>43</v>
       </c>
       <c r="B64" s="5" t="s">
@@ -1640,7 +1688,7 @@
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A65" s="21"/>
+      <c r="A65" s="22"/>
       <c r="B65" s="5" t="s">
         <v>0</v>
       </c>
@@ -1649,7 +1697,7 @@
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A66" s="21"/>
+      <c r="A66" s="22"/>
       <c r="B66" s="5" t="s">
         <v>2</v>
       </c>
@@ -1658,7 +1706,7 @@
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A67" s="21"/>
+      <c r="A67" s="22"/>
       <c r="B67" s="5" t="s">
         <v>9</v>
       </c>
@@ -1667,7 +1715,7 @@
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A68" s="21"/>
+      <c r="A68" s="22"/>
       <c r="B68" s="5" t="s">
         <v>3</v>
       </c>
@@ -1676,7 +1724,7 @@
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A69" s="21"/>
+      <c r="A69" s="22"/>
       <c r="B69" s="5" t="s">
         <v>1</v>
       </c>
@@ -1685,7 +1733,7 @@
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A70" s="21"/>
+      <c r="A70" s="22"/>
       <c r="B70" s="5" t="s">
         <v>85</v>
       </c>
@@ -1697,7 +1745,7 @@
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A71" s="21"/>
+      <c r="A71" s="22"/>
       <c r="B71" s="5" t="s">
         <v>21</v>
       </c>
@@ -1706,7 +1754,7 @@
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A72" s="21"/>
+      <c r="A72" s="22"/>
       <c r="B72" s="5" t="s">
         <v>15</v>
       </c>
@@ -1715,7 +1763,7 @@
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A73" s="21"/>
+      <c r="A73" s="22"/>
       <c r="B73" s="5" t="s">
         <v>81</v>
       </c>
@@ -1727,7 +1775,7 @@
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A74" s="21"/>
+      <c r="A74" s="22"/>
       <c r="B74" s="5" t="s">
         <v>82</v>
       </c>
@@ -1739,7 +1787,7 @@
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A75" s="21"/>
+      <c r="A75" s="22"/>
       <c r="B75" s="5" t="s">
         <v>64</v>
       </c>
@@ -1748,7 +1796,7 @@
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A76" s="21"/>
+      <c r="A76" s="22"/>
       <c r="B76" s="5" t="s">
         <v>65</v>
       </c>
@@ -1757,7 +1805,7 @@
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A77" s="21"/>
+      <c r="A77" s="22"/>
       <c r="B77" s="5" t="s">
         <v>66</v>
       </c>
@@ -1766,7 +1814,7 @@
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A78" s="14" t="s">
+      <c r="A78" s="15" t="s">
         <v>47</v>
       </c>
       <c r="B78" s="7" t="s">
@@ -1777,7 +1825,7 @@
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A79" s="15"/>
+      <c r="A79" s="16"/>
       <c r="B79" s="7" t="s">
         <v>49</v>
       </c>
@@ -1786,7 +1834,7 @@
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A80" s="15"/>
+      <c r="A80" s="16"/>
       <c r="B80" s="7" t="s">
         <v>50</v>
       </c>
@@ -1795,7 +1843,7 @@
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A81" s="15"/>
+      <c r="A81" s="16"/>
       <c r="B81" s="7" t="s">
         <v>86</v>
       </c>
@@ -1804,7 +1852,7 @@
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A82" s="15"/>
+      <c r="A82" s="16"/>
       <c r="B82" s="7" t="s">
         <v>87</v>
       </c>
@@ -1813,7 +1861,7 @@
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A83" s="15"/>
+      <c r="A83" s="16"/>
       <c r="B83" s="7" t="s">
         <v>74</v>
       </c>
@@ -1822,7 +1870,7 @@
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A84" s="15"/>
+      <c r="A84" s="16"/>
       <c r="B84" s="7" t="s">
         <v>75</v>
       </c>
@@ -1831,7 +1879,7 @@
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A85" s="15"/>
+      <c r="A85" s="16"/>
       <c r="B85" s="7" t="s">
         <v>76</v>
       </c>
@@ -1840,7 +1888,7 @@
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A86" s="15"/>
+      <c r="A86" s="16"/>
       <c r="B86" s="7" t="s">
         <v>77</v>
       </c>
@@ -1849,7 +1897,7 @@
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A87" s="15"/>
+      <c r="A87" s="16"/>
       <c r="B87" s="7" t="s">
         <v>72</v>
       </c>
@@ -1858,7 +1906,7 @@
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A88" s="14" t="s">
+      <c r="A88" s="15" t="s">
         <v>70</v>
       </c>
       <c r="B88" s="5" t="s">
@@ -1869,7 +1917,7 @@
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A89" s="15"/>
+      <c r="A89" s="16"/>
       <c r="B89" s="8" t="s">
         <v>72</v>
       </c>
@@ -1878,7 +1926,7 @@
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A90" s="14" t="s">
+      <c r="A90" s="15" t="s">
         <v>78</v>
       </c>
       <c r="B90" s="5" t="s">
@@ -1889,7 +1937,7 @@
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A91" s="15"/>
+      <c r="A91" s="16"/>
       <c r="B91" s="5" t="s">
         <v>51</v>
       </c>
@@ -1898,7 +1946,7 @@
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A92" s="16"/>
+      <c r="A92" s="17"/>
       <c r="B92" s="5" t="s">
         <v>72</v>
       </c>
@@ -1932,10 +1980,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H34"/>
+  <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1976,7 +2024,7 @@
       <c r="B2" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="14"/>
+      <c r="C2" s="22"/>
       <c r="D2" s="5" t="s">
         <v>109</v>
       </c>
@@ -1991,7 +2039,7 @@
       <c r="B3" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="C3" s="15"/>
+      <c r="C3" s="22"/>
       <c r="D3" s="5" t="s">
         <v>110</v>
       </c>
@@ -2006,7 +2054,7 @@
       <c r="B4" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="C4" s="15"/>
+      <c r="C4" s="22"/>
       <c r="D4" s="5" t="s">
         <v>117</v>
       </c>
@@ -2023,7 +2071,7 @@
       <c r="B5" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="C5" s="15"/>
+      <c r="C5" s="22"/>
       <c r="D5" s="5" t="s">
         <v>119</v>
       </c>
@@ -2040,7 +2088,7 @@
       <c r="B6" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="C6" s="15"/>
+      <c r="C6" s="22"/>
       <c r="D6" s="5" t="s">
         <v>120</v>
       </c>
@@ -2059,7 +2107,7 @@
       <c r="B7" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="C7" s="15"/>
+      <c r="C7" s="22"/>
       <c r="D7" s="5" t="s">
         <v>111</v>
       </c>
@@ -2078,7 +2126,7 @@
       <c r="B8" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="C8" s="15"/>
+      <c r="C8" s="22"/>
       <c r="D8" s="5" t="s">
         <v>112</v>
       </c>
@@ -2095,52 +2143,50 @@
         <v>92</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="C9" s="15"/>
-      <c r="D9" s="7" t="s">
-        <v>138</v>
-      </c>
-      <c r="E9" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="22"/>
+      <c r="D9" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="E9" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="F9" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="G9" s="7"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>92</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="C10" s="15"/>
-      <c r="D10" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="F10" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="C10" s="22"/>
+      <c r="D10" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="F10" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="G10" s="5"/>
+      <c r="G10" s="7"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>92</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="C11" s="16"/>
+        <v>98</v>
+      </c>
+      <c r="C11" s="22"/>
       <c r="D11" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>80</v>
+        <v>41</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>88</v>
@@ -2148,334 +2194,326 @@
       <c r="G11" s="5"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="22" t="s">
+      <c r="A12" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="22"/>
+      <c r="D12" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="C13" s="22"/>
+      <c r="D13" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="G13" s="5"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="C14" s="22"/>
+      <c r="D14" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="C15" s="23" t="s">
+        <v>133</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="G15" s="7"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="C16" s="23"/>
+      <c r="D16" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="G16" s="7"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="C17" s="23"/>
+      <c r="D17" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="E17" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="G17" s="14"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="C18" s="23"/>
+      <c r="D18" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="C12" s="24" t="s">
-        <v>134</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="E12" s="7" t="s">
+      <c r="E18" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="F12" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="G12" s="7"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="22" t="s">
-        <v>92</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="C13" s="25"/>
-      <c r="D13" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="G13" s="7"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="22" t="s">
-        <v>92</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="C14" s="26"/>
-      <c r="D14" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="5" t="s">
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="5" t="s">
         <v>91</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="G15" s="5"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C16" s="15"/>
-      <c r="D16" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="G16" s="5"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" s="15"/>
-      <c r="D17" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="G17" s="5"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C18" s="15"/>
-      <c r="D18" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="G18" s="5"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" s="5" t="s">
-        <v>92</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="15"/>
+      <c r="C19" s="22" t="s">
+        <v>107</v>
+      </c>
       <c r="D19" s="5" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="F19" s="5"/>
+        <v>89</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>90</v>
+      </c>
       <c r="G19" s="5"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="15"/>
+      <c r="C20" s="22"/>
       <c r="D20" s="5" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="F20" s="5"/>
+        <v>89</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>90</v>
+      </c>
       <c r="G20" s="5"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
         <v>91</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C21" s="16"/>
-      <c r="D21" s="23" t="s">
-        <v>140</v>
-      </c>
-      <c r="E21" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="F21" s="23"/>
-      <c r="G21" s="23"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C21" s="22"/>
+      <c r="D21" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="G21" s="5"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
         <v>91</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C22" s="14" t="s">
-        <v>115</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C22" s="22"/>
+      <c r="D22" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="G22" s="5"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C23" s="15"/>
-      <c r="D23" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C23" s="22"/>
+      <c r="D23" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C24" s="16"/>
+      <c r="C24" s="22"/>
       <c r="D24" s="5" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>90</v>
-      </c>
+        <v>106</v>
+      </c>
+      <c r="F24" s="5"/>
       <c r="G24" s="5"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
         <v>91</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C25" s="14" t="s">
-        <v>122</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="F25" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="G25" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+      <c r="C25" s="22"/>
+      <c r="D25" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="E25" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="C26" s="15"/>
-      <c r="D26" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="E26" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="F26" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="G26" s="5"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+      <c r="C26" s="22" t="s">
+        <v>115</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="C27" s="15"/>
-      <c r="D27" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="G27" s="5"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+      <c r="C27" s="22"/>
+      <c r="D27" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C28" s="15"/>
+        <v>16</v>
+      </c>
+      <c r="C28" s="22"/>
       <c r="D28" s="5" t="s">
-        <v>128</v>
+        <v>103</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>125</v>
+        <v>89</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="G28" s="5" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+        <v>90</v>
+      </c>
+      <c r="G28" s="5"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
         <v>91</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="C29" s="15"/>
+        <v>31</v>
+      </c>
+      <c r="C29" s="22" t="s">
+        <v>122</v>
+      </c>
       <c r="D29" s="5" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="E29" s="5" t="s">
         <v>125</v>
@@ -2484,101 +2522,340 @@
         <v>124</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
         <v>92</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="C30" s="15"/>
-      <c r="D30" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="E30" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="C30" s="22"/>
+      <c r="D30" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="F30" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="F30" s="7"/>
-      <c r="G30" s="7"/>
-      <c r="H30" s="3" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G30" s="5"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
         <v>92</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C31" s="16"/>
-      <c r="D31" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="E31" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="F31" s="7"/>
-      <c r="G31" s="7"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+        <v>131</v>
+      </c>
+      <c r="C31" s="22"/>
+      <c r="D31" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="G31" s="5"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
         <v>92</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="C32" s="14" t="s">
-        <v>143</v>
-      </c>
-      <c r="D32" s="23" t="s">
-        <v>105</v>
-      </c>
-      <c r="E32" s="23"/>
-      <c r="F32" s="23"/>
-      <c r="G32" s="23"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+      <c r="C32" s="22"/>
+      <c r="D32" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="G32" s="5" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="C33" s="15"/>
-      <c r="D33" s="23" t="s">
-        <v>113</v>
-      </c>
-      <c r="E33" s="23"/>
-      <c r="F33" s="23"/>
-      <c r="G33" s="23"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+        <v>57</v>
+      </c>
+      <c r="C33" s="22"/>
+      <c r="D33" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="5" t="s">
         <v>92</v>
       </c>
       <c r="B34" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="C34" s="22"/>
+      <c r="D34" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
+      <c r="H34" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C35" s="22"/>
+      <c r="D35" s="24" t="s">
+        <v>151</v>
+      </c>
+      <c r="E35" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="F35" s="24" t="s">
+        <v>152</v>
+      </c>
+      <c r="G35" s="24"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C36" s="22"/>
+      <c r="D36" s="24" t="s">
+        <v>156</v>
+      </c>
+      <c r="E36" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="F36" s="24" t="s">
+        <v>152</v>
+      </c>
+      <c r="G36" s="24"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C37" s="22"/>
+      <c r="D37" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="E37" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="F37" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G37" s="7"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C38" s="22"/>
+      <c r="D38" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="E38" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="F38" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G38" s="7"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C39" s="22"/>
+      <c r="D39" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="E39" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="F39" s="7"/>
+      <c r="G39" s="7"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="C40" s="22" t="s">
+        <v>142</v>
+      </c>
+      <c r="D40" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="E40" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="F40" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="G40" s="14" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C41" s="22"/>
+      <c r="D41" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="E41" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="F41" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="G41" s="14"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A42" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="C42" s="22"/>
+      <c r="D42" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="E42" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="F42" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="G42" s="14"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A43" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B43" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="C34" s="16"/>
-      <c r="D34" s="23" t="s">
+      <c r="C43" s="22"/>
+      <c r="D43" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="E34" s="23"/>
-      <c r="F34" s="23"/>
-      <c r="G34" s="23"/>
+      <c r="E43" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="F43" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="G43" s="14" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A44" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C44" s="22" t="s">
+        <v>147</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="E44" s="5"/>
+      <c r="F44" s="5"/>
+      <c r="G44" s="5"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A45" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C45" s="22"/>
+      <c r="D45" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="E45" s="5"/>
+      <c r="F45" s="5"/>
+      <c r="G45" s="5"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A46" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="C46" s="22"/>
+      <c r="D46" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="E46" s="7"/>
+      <c r="F46" s="7"/>
+      <c r="G46" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="C2:C11"/>
-    <mergeCell ref="C32:C34"/>
-    <mergeCell ref="C25:C31"/>
-    <mergeCell ref="C12:C14"/>
-    <mergeCell ref="C22:C24"/>
-    <mergeCell ref="C15:C21"/>
+  <mergeCells count="7">
+    <mergeCell ref="C44:C46"/>
+    <mergeCell ref="C2:C14"/>
+    <mergeCell ref="C40:C43"/>
+    <mergeCell ref="C29:C39"/>
+    <mergeCell ref="C15:C18"/>
+    <mergeCell ref="C26:C28"/>
+    <mergeCell ref="C19:C25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
update userservices for join and order activities
</commit_message>
<xml_diff>
--- a/document/gpe_model.xlsx
+++ b/document/gpe_model.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="960" yWindow="440" windowWidth="26360" windowHeight="14920" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="860" yWindow="440" windowWidth="26460" windowHeight="14920" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="dictionary" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="173">
   <si>
     <t>name</t>
   </si>
@@ -511,6 +511,42 @@
   </si>
   <si>
     <t>/vdetail</t>
+  </si>
+  <si>
+    <t>/gusr</t>
+  </si>
+  <si>
+    <t>/orderlist</t>
+  </si>
+  <si>
+    <t>/memberlist</t>
+  </si>
+  <si>
+    <t>usid</t>
+  </si>
+  <si>
+    <t>pd</t>
+  </si>
+  <si>
+    <t>actid</t>
+  </si>
+  <si>
+    <t>List&lt;ActOds&gt;</t>
+  </si>
+  <si>
+    <t>/book</t>
+  </si>
+  <si>
+    <t>act</t>
+  </si>
+  <si>
+    <t>count</t>
+  </si>
+  <si>
+    <t>/pay</t>
+  </si>
+  <si>
+    <t>ord</t>
   </si>
 </sst>
 </file>
@@ -697,6 +733,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -723,9 +762,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1035,7 +1071,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="16" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -1046,7 +1082,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="16"/>
+      <c r="A3" s="17"/>
       <c r="B3" s="5" t="s">
         <v>0</v>
       </c>
@@ -1058,7 +1094,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="16"/>
+      <c r="A4" s="17"/>
       <c r="B4" s="5" t="s">
         <v>1</v>
       </c>
@@ -1067,7 +1103,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="16"/>
+      <c r="A5" s="17"/>
       <c r="B5" s="5" t="s">
         <v>2</v>
       </c>
@@ -1076,7 +1112,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="16"/>
+      <c r="A6" s="17"/>
       <c r="B6" s="5" t="s">
         <v>3</v>
       </c>
@@ -1088,7 +1124,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="16"/>
+      <c r="A7" s="17"/>
       <c r="B7" s="5" t="s">
         <v>81</v>
       </c>
@@ -1097,7 +1133,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="16"/>
+      <c r="A8" s="17"/>
       <c r="B8" s="5" t="s">
         <v>40</v>
       </c>
@@ -1106,7 +1142,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="16"/>
+      <c r="A9" s="17"/>
       <c r="B9" s="5" t="s">
         <v>21</v>
       </c>
@@ -1115,7 +1151,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="17"/>
+      <c r="A10" s="18"/>
       <c r="B10" s="5" t="s">
         <v>52</v>
       </c>
@@ -1124,7 +1160,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="15" t="s">
+      <c r="A11" s="16" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="5" t="s">
@@ -1135,7 +1171,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="16"/>
+      <c r="A12" s="17"/>
       <c r="B12" s="5" t="s">
         <v>5</v>
       </c>
@@ -1144,7 +1180,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="16"/>
+      <c r="A13" s="17"/>
       <c r="B13" s="5" t="s">
         <v>7</v>
       </c>
@@ -1156,7 +1192,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="16"/>
+      <c r="A14" s="17"/>
       <c r="B14" s="5" t="s">
         <v>8</v>
       </c>
@@ -1165,7 +1201,7 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="16"/>
+      <c r="A15" s="17"/>
       <c r="B15" s="5" t="s">
         <v>9</v>
       </c>
@@ -1174,7 +1210,7 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="17"/>
+      <c r="A16" s="18"/>
       <c r="B16" s="5" t="s">
         <v>82</v>
       </c>
@@ -1186,7 +1222,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="15" t="s">
+      <c r="A17" s="16" t="s">
         <v>16</v>
       </c>
       <c r="B17" s="5" t="s">
@@ -1197,7 +1233,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="16"/>
+      <c r="A18" s="17"/>
       <c r="B18" s="5" t="s">
         <v>11</v>
       </c>
@@ -1206,7 +1242,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="16"/>
+      <c r="A19" s="17"/>
       <c r="B19" s="5" t="s">
         <v>12</v>
       </c>
@@ -1218,7 +1254,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="16"/>
+      <c r="A20" s="17"/>
       <c r="B20" s="5" t="s">
         <v>13</v>
       </c>
@@ -1227,7 +1263,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="16"/>
+      <c r="A21" s="17"/>
       <c r="B21" s="5" t="s">
         <v>14</v>
       </c>
@@ -1239,7 +1275,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="16"/>
+      <c r="A22" s="17"/>
       <c r="B22" s="5" t="s">
         <v>9</v>
       </c>
@@ -1248,7 +1284,7 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="16"/>
+      <c r="A23" s="17"/>
       <c r="B23" s="5" t="s">
         <v>15</v>
       </c>
@@ -1257,7 +1293,7 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="16"/>
+      <c r="A24" s="17"/>
       <c r="B24" s="5" t="s">
         <v>83</v>
       </c>
@@ -1269,7 +1305,7 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="16"/>
+      <c r="A25" s="17"/>
       <c r="B25" s="5" t="s">
         <v>84</v>
       </c>
@@ -1281,7 +1317,7 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="16"/>
+      <c r="A26" s="17"/>
       <c r="B26" s="5" t="s">
         <v>0</v>
       </c>
@@ -1290,7 +1326,7 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="16"/>
+      <c r="A27" s="17"/>
       <c r="B27" s="5" t="s">
         <v>48</v>
       </c>
@@ -1299,7 +1335,7 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="17"/>
+      <c r="A28" s="18"/>
       <c r="B28" s="5" t="s">
         <v>71</v>
       </c>
@@ -1308,7 +1344,7 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="15" t="s">
+      <c r="A29" s="16" t="s">
         <v>17</v>
       </c>
       <c r="B29" s="5" t="s">
@@ -1319,7 +1355,7 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="16"/>
+      <c r="A30" s="17"/>
       <c r="B30" s="5" t="s">
         <v>0</v>
       </c>
@@ -1331,7 +1367,7 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="16"/>
+      <c r="A31" s="17"/>
       <c r="B31" s="5" t="s">
         <v>18</v>
       </c>
@@ -1340,7 +1376,7 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="16"/>
+      <c r="A32" s="17"/>
       <c r="B32" s="5" t="s">
         <v>19</v>
       </c>
@@ -1352,7 +1388,7 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="16"/>
+      <c r="A33" s="17"/>
       <c r="B33" s="5" t="s">
         <v>20</v>
       </c>
@@ -1361,7 +1397,7 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" s="17"/>
+      <c r="A34" s="18"/>
       <c r="B34" s="5" t="s">
         <v>21</v>
       </c>
@@ -1370,7 +1406,7 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="15" t="s">
+      <c r="A35" s="16" t="s">
         <v>22</v>
       </c>
       <c r="B35" s="5" t="s">
@@ -1381,7 +1417,7 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="16"/>
+      <c r="A36" s="17"/>
       <c r="B36" s="5" t="s">
         <v>0</v>
       </c>
@@ -1393,7 +1429,7 @@
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="17"/>
+      <c r="A37" s="18"/>
       <c r="B37" s="5" t="s">
         <v>21</v>
       </c>
@@ -1402,7 +1438,7 @@
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="15" t="s">
+      <c r="A38" s="16" t="s">
         <v>24</v>
       </c>
       <c r="B38" s="5" t="s">
@@ -1413,7 +1449,7 @@
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" s="16"/>
+      <c r="A39" s="17"/>
       <c r="B39" s="5" t="s">
         <v>82</v>
       </c>
@@ -1425,7 +1461,7 @@
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40" s="16"/>
+      <c r="A40" s="17"/>
       <c r="B40" s="5" t="s">
         <v>7</v>
       </c>
@@ -1437,7 +1473,7 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" s="17"/>
+      <c r="A41" s="18"/>
       <c r="B41" s="5" t="s">
         <v>25</v>
       </c>
@@ -1446,7 +1482,7 @@
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" s="15" t="s">
+      <c r="A42" s="16" t="s">
         <v>26</v>
       </c>
       <c r="B42" s="5" t="s">
@@ -1455,42 +1491,42 @@
       <c r="C42" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="D42" s="21" t="s">
+      <c r="D42" s="22" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" s="16"/>
+      <c r="A43" s="17"/>
       <c r="B43" s="5" t="s">
         <v>28</v>
       </c>
       <c r="C43" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="D43" s="21"/>
+      <c r="D43" s="22"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" s="16"/>
+      <c r="A44" s="17"/>
       <c r="B44" s="5" t="s">
         <v>29</v>
       </c>
       <c r="C44" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="D44" s="21"/>
+      <c r="D44" s="22"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="17"/>
+      <c r="A45" s="18"/>
       <c r="B45" s="5" t="s">
         <v>30</v>
       </c>
       <c r="C45" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="D45" s="21"/>
+      <c r="D45" s="22"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" s="15" t="s">
+      <c r="A46" s="16" t="s">
         <v>31</v>
       </c>
       <c r="B46" s="5" t="s">
@@ -1501,7 +1537,7 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47" s="16"/>
+      <c r="A47" s="17"/>
       <c r="B47" s="5" t="s">
         <v>32</v>
       </c>
@@ -1513,7 +1549,7 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A48" s="17"/>
+      <c r="A48" s="18"/>
       <c r="B48" s="5" t="s">
         <v>25</v>
       </c>
@@ -1522,7 +1558,7 @@
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" s="15" t="s">
+      <c r="A49" s="16" t="s">
         <v>33</v>
       </c>
       <c r="B49" s="5" t="s">
@@ -1533,7 +1569,7 @@
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50" s="16"/>
+      <c r="A50" s="17"/>
       <c r="B50" s="5" t="s">
         <v>34</v>
       </c>
@@ -1542,7 +1578,7 @@
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51" s="16"/>
+      <c r="A51" s="17"/>
       <c r="B51" s="5" t="s">
         <v>35</v>
       </c>
@@ -1554,7 +1590,7 @@
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A52" s="17"/>
+      <c r="A52" s="18"/>
       <c r="B52" s="5" t="s">
         <v>36</v>
       </c>
@@ -1566,7 +1602,7 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A53" s="18" t="s">
+      <c r="A53" s="19" t="s">
         <v>37</v>
       </c>
       <c r="B53" s="10" t="s">
@@ -1577,7 +1613,7 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A54" s="19"/>
+      <c r="A54" s="20"/>
       <c r="B54" s="10" t="s">
         <v>38</v>
       </c>
@@ -1586,7 +1622,7 @@
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A55" s="19"/>
+      <c r="A55" s="20"/>
       <c r="B55" s="10" t="s">
         <v>39</v>
       </c>
@@ -1595,7 +1631,7 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56" s="20"/>
+      <c r="A56" s="21"/>
       <c r="B56" s="10" t="s">
         <v>40</v>
       </c>
@@ -1604,7 +1640,7 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A57" s="15" t="s">
+      <c r="A57" s="16" t="s">
         <v>6</v>
       </c>
       <c r="B57" s="5" t="s">
@@ -1615,7 +1651,7 @@
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A58" s="16"/>
+      <c r="A58" s="17"/>
       <c r="B58" s="5" t="s">
         <v>0</v>
       </c>
@@ -1627,7 +1663,7 @@
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59" s="16"/>
+      <c r="A59" s="17"/>
       <c r="B59" s="5" t="s">
         <v>41</v>
       </c>
@@ -1636,7 +1672,7 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A60" s="17"/>
+      <c r="A60" s="18"/>
       <c r="B60" s="5" t="s">
         <v>21</v>
       </c>
@@ -1645,7 +1681,7 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A61" s="15" t="s">
+      <c r="A61" s="16" t="s">
         <v>42</v>
       </c>
       <c r="B61" s="5" t="s">
@@ -1656,7 +1692,7 @@
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A62" s="16"/>
+      <c r="A62" s="17"/>
       <c r="B62" s="5" t="s">
         <v>0</v>
       </c>
@@ -1668,7 +1704,7 @@
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A63" s="17"/>
+      <c r="A63" s="18"/>
       <c r="B63" s="5" t="s">
         <v>21</v>
       </c>
@@ -1677,7 +1713,7 @@
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A64" s="22" t="s">
+      <c r="A64" s="23" t="s">
         <v>43</v>
       </c>
       <c r="B64" s="5" t="s">
@@ -1688,7 +1724,7 @@
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A65" s="22"/>
+      <c r="A65" s="23"/>
       <c r="B65" s="5" t="s">
         <v>0</v>
       </c>
@@ -1697,7 +1733,7 @@
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A66" s="22"/>
+      <c r="A66" s="23"/>
       <c r="B66" s="5" t="s">
         <v>2</v>
       </c>
@@ -1706,7 +1742,7 @@
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A67" s="22"/>
+      <c r="A67" s="23"/>
       <c r="B67" s="5" t="s">
         <v>9</v>
       </c>
@@ -1715,7 +1751,7 @@
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A68" s="22"/>
+      <c r="A68" s="23"/>
       <c r="B68" s="5" t="s">
         <v>3</v>
       </c>
@@ -1724,7 +1760,7 @@
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A69" s="22"/>
+      <c r="A69" s="23"/>
       <c r="B69" s="5" t="s">
         <v>1</v>
       </c>
@@ -1733,7 +1769,7 @@
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A70" s="22"/>
+      <c r="A70" s="23"/>
       <c r="B70" s="5" t="s">
         <v>85</v>
       </c>
@@ -1745,7 +1781,7 @@
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A71" s="22"/>
+      <c r="A71" s="23"/>
       <c r="B71" s="5" t="s">
         <v>21</v>
       </c>
@@ -1754,7 +1790,7 @@
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A72" s="22"/>
+      <c r="A72" s="23"/>
       <c r="B72" s="5" t="s">
         <v>15</v>
       </c>
@@ -1763,7 +1799,7 @@
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A73" s="22"/>
+      <c r="A73" s="23"/>
       <c r="B73" s="5" t="s">
         <v>81</v>
       </c>
@@ -1775,7 +1811,7 @@
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A74" s="22"/>
+      <c r="A74" s="23"/>
       <c r="B74" s="5" t="s">
         <v>82</v>
       </c>
@@ -1787,7 +1823,7 @@
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A75" s="22"/>
+      <c r="A75" s="23"/>
       <c r="B75" s="5" t="s">
         <v>64</v>
       </c>
@@ -1796,7 +1832,7 @@
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A76" s="22"/>
+      <c r="A76" s="23"/>
       <c r="B76" s="5" t="s">
         <v>65</v>
       </c>
@@ -1805,7 +1841,7 @@
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A77" s="22"/>
+      <c r="A77" s="23"/>
       <c r="B77" s="5" t="s">
         <v>66</v>
       </c>
@@ -1814,7 +1850,7 @@
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A78" s="15" t="s">
+      <c r="A78" s="16" t="s">
         <v>47</v>
       </c>
       <c r="B78" s="7" t="s">
@@ -1825,7 +1861,7 @@
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A79" s="16"/>
+      <c r="A79" s="17"/>
       <c r="B79" s="7" t="s">
         <v>49</v>
       </c>
@@ -1834,7 +1870,7 @@
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A80" s="16"/>
+      <c r="A80" s="17"/>
       <c r="B80" s="7" t="s">
         <v>50</v>
       </c>
@@ -1843,7 +1879,7 @@
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A81" s="16"/>
+      <c r="A81" s="17"/>
       <c r="B81" s="7" t="s">
         <v>86</v>
       </c>
@@ -1852,7 +1888,7 @@
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A82" s="16"/>
+      <c r="A82" s="17"/>
       <c r="B82" s="7" t="s">
         <v>87</v>
       </c>
@@ -1861,7 +1897,7 @@
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A83" s="16"/>
+      <c r="A83" s="17"/>
       <c r="B83" s="7" t="s">
         <v>74</v>
       </c>
@@ -1870,7 +1906,7 @@
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A84" s="16"/>
+      <c r="A84" s="17"/>
       <c r="B84" s="7" t="s">
         <v>75</v>
       </c>
@@ -1879,7 +1915,7 @@
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A85" s="16"/>
+      <c r="A85" s="17"/>
       <c r="B85" s="7" t="s">
         <v>76</v>
       </c>
@@ -1888,7 +1924,7 @@
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A86" s="16"/>
+      <c r="A86" s="17"/>
       <c r="B86" s="7" t="s">
         <v>77</v>
       </c>
@@ -1897,7 +1933,7 @@
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A87" s="16"/>
+      <c r="A87" s="17"/>
       <c r="B87" s="7" t="s">
         <v>72</v>
       </c>
@@ -1906,7 +1942,7 @@
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A88" s="15" t="s">
+      <c r="A88" s="16" t="s">
         <v>70</v>
       </c>
       <c r="B88" s="5" t="s">
@@ -1917,7 +1953,7 @@
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A89" s="16"/>
+      <c r="A89" s="17"/>
       <c r="B89" s="8" t="s">
         <v>72</v>
       </c>
@@ -1926,7 +1962,7 @@
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A90" s="15" t="s">
+      <c r="A90" s="16" t="s">
         <v>78</v>
       </c>
       <c r="B90" s="5" t="s">
@@ -1937,7 +1973,7 @@
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A91" s="16"/>
+      <c r="A91" s="17"/>
       <c r="B91" s="5" t="s">
         <v>51</v>
       </c>
@@ -1946,7 +1982,7 @@
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A92" s="17"/>
+      <c r="A92" s="18"/>
       <c r="B92" s="5" t="s">
         <v>72</v>
       </c>
@@ -1980,10 +2016,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H46"/>
+  <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="226" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2024,7 +2060,7 @@
       <c r="B2" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="22"/>
+      <c r="C2" s="23"/>
       <c r="D2" s="5" t="s">
         <v>109</v>
       </c>
@@ -2039,7 +2075,7 @@
       <c r="B3" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="C3" s="22"/>
+      <c r="C3" s="23"/>
       <c r="D3" s="5" t="s">
         <v>110</v>
       </c>
@@ -2054,7 +2090,7 @@
       <c r="B4" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="C4" s="22"/>
+      <c r="C4" s="23"/>
       <c r="D4" s="5" t="s">
         <v>117</v>
       </c>
@@ -2071,7 +2107,7 @@
       <c r="B5" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="C5" s="22"/>
+      <c r="C5" s="23"/>
       <c r="D5" s="5" t="s">
         <v>119</v>
       </c>
@@ -2088,7 +2124,7 @@
       <c r="B6" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="C6" s="22"/>
+      <c r="C6" s="23"/>
       <c r="D6" s="5" t="s">
         <v>120</v>
       </c>
@@ -2107,7 +2143,7 @@
       <c r="B7" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="C7" s="22"/>
+      <c r="C7" s="23"/>
       <c r="D7" s="5" t="s">
         <v>111</v>
       </c>
@@ -2126,7 +2162,7 @@
       <c r="B8" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="C8" s="22"/>
+      <c r="C8" s="23"/>
       <c r="D8" s="5" t="s">
         <v>112</v>
       </c>
@@ -2145,7 +2181,7 @@
       <c r="B9" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C9" s="22"/>
+      <c r="C9" s="23"/>
       <c r="D9" s="5" t="s">
         <v>159</v>
       </c>
@@ -2162,7 +2198,7 @@
       <c r="B10" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="C10" s="22"/>
+      <c r="C10" s="23"/>
       <c r="D10" s="7" t="s">
         <v>137</v>
       </c>
@@ -2181,7 +2217,7 @@
       <c r="B11" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="C11" s="22"/>
+      <c r="C11" s="23"/>
       <c r="D11" s="5" t="s">
         <v>113</v>
       </c>
@@ -2200,7 +2236,7 @@
       <c r="B12" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="22"/>
+      <c r="C12" s="23"/>
       <c r="D12" s="5" t="s">
         <v>160</v>
       </c>
@@ -2217,7 +2253,7 @@
       <c r="B13" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="C13" s="22"/>
+      <c r="C13" s="23"/>
       <c r="D13" s="5" t="s">
         <v>114</v>
       </c>
@@ -2236,7 +2272,7 @@
       <c r="B14" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="C14" s="22"/>
+      <c r="C14" s="23"/>
       <c r="D14" s="5" t="s">
         <v>119</v>
       </c>
@@ -2253,7 +2289,7 @@
       <c r="B15" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="C15" s="23" t="s">
+      <c r="C15" s="24" t="s">
         <v>133</v>
       </c>
       <c r="D15" s="7" t="s">
@@ -2274,7 +2310,7 @@
       <c r="B16" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="C16" s="23"/>
+      <c r="C16" s="24"/>
       <c r="D16" s="7" t="s">
         <v>111</v>
       </c>
@@ -2293,7 +2329,7 @@
       <c r="B17" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="C17" s="23"/>
+      <c r="C17" s="24"/>
       <c r="D17" s="14" t="s">
         <v>144</v>
       </c>
@@ -2312,7 +2348,7 @@
       <c r="B18" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="C18" s="23"/>
+      <c r="C18" s="24"/>
       <c r="D18" s="7" t="s">
         <v>135</v>
       </c>
@@ -2329,7 +2365,7 @@
       <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="22" t="s">
+      <c r="C19" s="23" t="s">
         <v>107</v>
       </c>
       <c r="D19" s="5" t="s">
@@ -2350,7 +2386,7 @@
       <c r="B20" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="22"/>
+      <c r="C20" s="23"/>
       <c r="D20" s="5" t="s">
         <v>101</v>
       </c>
@@ -2369,7 +2405,7 @@
       <c r="B21" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C21" s="22"/>
+      <c r="C21" s="23"/>
       <c r="D21" s="5" t="s">
         <v>102</v>
       </c>
@@ -2388,7 +2424,7 @@
       <c r="B22" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C22" s="22"/>
+      <c r="C22" s="23"/>
       <c r="D22" s="5" t="s">
         <v>103</v>
       </c>
@@ -2407,7 +2443,7 @@
       <c r="B23" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C23" s="22"/>
+      <c r="C23" s="23"/>
       <c r="D23" s="5" t="s">
         <v>104</v>
       </c>
@@ -2424,7 +2460,7 @@
       <c r="B24" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C24" s="22"/>
+      <c r="C24" s="23"/>
       <c r="D24" s="5" t="s">
         <v>105</v>
       </c>
@@ -2436,20 +2472,22 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C25" s="22"/>
-      <c r="D25" s="14" t="s">
-        <v>139</v>
-      </c>
-      <c r="E25" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="F25" s="14"/>
-      <c r="G25" s="14"/>
+      <c r="C25" s="23"/>
+      <c r="D25" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="G25" s="5"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
@@ -2458,15 +2496,15 @@
       <c r="B26" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C26" s="22" t="s">
-        <v>115</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="7"/>
+      <c r="C26" s="23"/>
+      <c r="D26" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="E26" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
@@ -2475,9 +2513,11 @@
       <c r="B27" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C27" s="22"/>
+      <c r="C27" s="23" t="s">
+        <v>115</v>
+      </c>
       <c r="D27" s="7" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E27" s="7"/>
       <c r="F27" s="7"/>
@@ -2490,59 +2530,55 @@
       <c r="B28" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C28" s="22"/>
-      <c r="D28" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="E28" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="F28" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="G28" s="5"/>
+      <c r="C28" s="23"/>
+      <c r="D28" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
         <v>91</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C29" s="22" t="s">
-        <v>122</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="C29" s="23"/>
       <c r="D29" s="5" t="s">
-        <v>123</v>
+        <v>103</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>125</v>
+        <v>89</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="G29" s="5" t="s">
-        <v>25</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="G29" s="5"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="C30" s="22"/>
+        <v>31</v>
+      </c>
+      <c r="C30" s="23" t="s">
+        <v>122</v>
+      </c>
       <c r="D30" s="5" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="E30" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="F30" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="F30" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="G30" s="5"/>
+      <c r="G30" s="5" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
@@ -2551,12 +2587,12 @@
       <c r="B31" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="C31" s="22"/>
+      <c r="C31" s="23"/>
       <c r="D31" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F31" s="5" t="s">
         <v>88</v>
@@ -2568,32 +2604,30 @@
         <v>92</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C32" s="22"/>
+        <v>131</v>
+      </c>
+      <c r="C32" s="23"/>
       <c r="D32" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E32" s="5" t="s">
         <v>125</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="G32" s="5" t="s">
-        <v>129</v>
-      </c>
+        <v>88</v>
+      </c>
+      <c r="G32" s="5"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C33" s="22"/>
+        <v>31</v>
+      </c>
+      <c r="C33" s="23"/>
       <c r="D33" s="5" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="E33" s="5" t="s">
         <v>125</v>
@@ -2607,78 +2641,82 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="C34" s="22"/>
-      <c r="D34" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="E34" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="F34" s="7"/>
-      <c r="G34" s="7"/>
-      <c r="H34" s="3" t="s">
-        <v>143</v>
+        <v>57</v>
+      </c>
+      <c r="C34" s="23"/>
+      <c r="D34" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="G34" s="5" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="5" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C35" s="22"/>
-      <c r="D35" s="24" t="s">
-        <v>151</v>
-      </c>
-      <c r="E35" s="24" t="s">
-        <v>89</v>
-      </c>
-      <c r="F35" s="24" t="s">
-        <v>152</v>
-      </c>
-      <c r="G35" s="24"/>
+        <v>141</v>
+      </c>
+      <c r="C35" s="23"/>
+      <c r="D35" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="E35" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="F35" s="7"/>
+      <c r="G35" s="7"/>
+      <c r="H35" s="3" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="5" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C36" s="22"/>
-      <c r="D36" s="24" t="s">
-        <v>156</v>
-      </c>
-      <c r="E36" s="24" t="s">
-        <v>89</v>
-      </c>
-      <c r="F36" s="24" t="s">
-        <v>152</v>
-      </c>
-      <c r="G36" s="24"/>
+        <v>167</v>
+      </c>
+      <c r="C36" s="23"/>
+      <c r="D36" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="E36" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="F36" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="G36" s="7" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="5" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C37" s="22"/>
+        <v>167</v>
+      </c>
+      <c r="C37" s="23"/>
       <c r="D37" s="7" t="s">
-        <v>153</v>
+        <v>163</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>89</v>
+        <v>166</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>155</v>
+        <v>88</v>
       </c>
       <c r="G37" s="7"/>
     </row>
@@ -2689,173 +2727,268 @@
       <c r="B38" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C38" s="22"/>
+      <c r="C38" s="23"/>
       <c r="D38" s="7" t="s">
-        <v>154</v>
+        <v>168</v>
       </c>
       <c r="E38" s="7" t="s">
         <v>89</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="G38" s="7"/>
+        <v>169</v>
+      </c>
+      <c r="G38" s="7" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C39" s="22"/>
+        <v>57</v>
+      </c>
+      <c r="C39" s="23"/>
       <c r="D39" s="7" t="s">
-        <v>135</v>
+        <v>171</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>80</v>
+        <v>172</v>
       </c>
       <c r="F39" s="7"/>
       <c r="G39" s="7"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="C40" s="22" t="s">
-        <v>142</v>
-      </c>
-      <c r="D40" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="E40" s="14" t="s">
-        <v>157</v>
-      </c>
-      <c r="F40" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="G40" s="14" t="s">
-        <v>88</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="C40" s="23"/>
+      <c r="D40" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="E40" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="F40" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="G40" s="15"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="C41" s="22"/>
-      <c r="D41" s="14" t="s">
-        <v>113</v>
-      </c>
-      <c r="E41" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="F41" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="G41" s="14"/>
+        <v>57</v>
+      </c>
+      <c r="C41" s="23"/>
+      <c r="D41" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="E41" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="F41" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="G41" s="15"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="C42" s="22"/>
-      <c r="D42" s="14" t="s">
-        <v>158</v>
-      </c>
-      <c r="E42" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="F42" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="G42" s="14"/>
+        <v>57</v>
+      </c>
+      <c r="C42" s="23"/>
+      <c r="D42" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="E42" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="F42" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G42" s="7"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="C43" s="22"/>
-      <c r="D43" s="14" t="s">
-        <v>111</v>
-      </c>
-      <c r="E43" s="14" t="s">
-        <v>157</v>
-      </c>
-      <c r="F43" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="G43" s="14" t="s">
-        <v>88</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="C43" s="23"/>
+      <c r="D43" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="E43" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="F43" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G43" s="7"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="5" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C44" s="22" t="s">
-        <v>147</v>
-      </c>
-      <c r="D44" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="E44" s="5"/>
-      <c r="F44" s="5"/>
-      <c r="G44" s="5"/>
+        <v>16</v>
+      </c>
+      <c r="C44" s="23"/>
+      <c r="D44" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="E44" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="F44" s="7"/>
+      <c r="G44" s="7"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="5" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C45" s="22"/>
-      <c r="D45" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="E45" s="5"/>
-      <c r="F45" s="5"/>
-      <c r="G45" s="5"/>
+        <v>141</v>
+      </c>
+      <c r="C45" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="D45" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="E45" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="F45" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="G45" s="7" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C46" s="23"/>
+      <c r="D46" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="E46" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="F46" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="G46" s="7"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A47" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="C47" s="23"/>
+      <c r="D47" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="E47" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="F47" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="G47" s="7"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A48" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C48" s="23"/>
+      <c r="D48" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="E48" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="F48" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="G48" s="7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A49" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="B46" s="5" t="s">
+      <c r="B49" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C49" s="23" t="s">
+        <v>147</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="E49" s="5"/>
+      <c r="F49" s="5"/>
+      <c r="G49" s="5"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A50" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C50" s="23"/>
+      <c r="D50" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="E50" s="5"/>
+      <c r="F50" s="5"/>
+      <c r="G50" s="5"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A51" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B51" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="C46" s="22"/>
-      <c r="D46" s="7" t="s">
+      <c r="C51" s="23"/>
+      <c r="D51" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="E46" s="7"/>
-      <c r="F46" s="7"/>
-      <c r="G46" s="7"/>
+      <c r="E51" s="7"/>
+      <c r="F51" s="7"/>
+      <c r="G51" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="C44:C46"/>
+    <mergeCell ref="C49:C51"/>
     <mergeCell ref="C2:C14"/>
-    <mergeCell ref="C40:C43"/>
-    <mergeCell ref="C29:C39"/>
+    <mergeCell ref="C45:C48"/>
+    <mergeCell ref="C30:C44"/>
     <mergeCell ref="C15:C18"/>
-    <mergeCell ref="C26:C28"/>
-    <mergeCell ref="C19:C25"/>
+    <mergeCell ref="C27:C29"/>
+    <mergeCell ref="C19:C26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
add running logging function and interface
</commit_message>
<xml_diff>
--- a/document/gpe_model.xlsx
+++ b/document/gpe_model.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="182">
   <si>
     <t>name</t>
   </si>
@@ -441,9 +441,6 @@
     <t>Activity</t>
   </si>
   <si>
-    <t>/csnews</t>
-  </si>
-  <si>
     <t>List&lt;Cnews&gt;</t>
   </si>
   <si>
@@ -547,6 +544,36 @@
   </si>
   <si>
     <t>ord</t>
+  </si>
+  <si>
+    <t>/cnews</t>
+  </si>
+  <si>
+    <t>/run</t>
+  </si>
+  <si>
+    <t>rmid</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t>/rp</t>
+  </si>
+  <si>
+    <t>/ad</t>
+  </si>
+  <si>
+    <t>RunningMan</t>
+  </si>
+  <si>
+    <t>List&lt;RunningMan&gt;</t>
+  </si>
+  <si>
+    <t>Running</t>
+  </si>
+  <si>
+    <t>List&lt;Running&gt;</t>
   </si>
 </sst>
 </file>
@@ -584,7 +611,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -606,12 +633,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -691,7 +712,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -733,8 +754,8 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -745,6 +766,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -752,12 +776,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1491,7 +1509,7 @@
       <c r="C42" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="D42" s="22" t="s">
+      <c r="D42" s="15" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1503,7 +1521,7 @@
       <c r="C43" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="D43" s="22"/>
+      <c r="D43" s="15"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="17"/>
@@ -1513,7 +1531,7 @@
       <c r="C44" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="D44" s="22"/>
+      <c r="D44" s="15"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="18"/>
@@ -1523,7 +1541,7 @@
       <c r="C45" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="D45" s="22"/>
+      <c r="D45" s="15"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="16" t="s">
@@ -1602,7 +1620,7 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A53" s="19" t="s">
+      <c r="A53" s="20" t="s">
         <v>37</v>
       </c>
       <c r="B53" s="10" t="s">
@@ -1613,7 +1631,7 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A54" s="20"/>
+      <c r="A54" s="21"/>
       <c r="B54" s="10" t="s">
         <v>38</v>
       </c>
@@ -1622,7 +1640,7 @@
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A55" s="20"/>
+      <c r="A55" s="21"/>
       <c r="B55" s="10" t="s">
         <v>39</v>
       </c>
@@ -1631,7 +1649,7 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56" s="21"/>
+      <c r="A56" s="22"/>
       <c r="B56" s="10" t="s">
         <v>40</v>
       </c>
@@ -1713,7 +1731,7 @@
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A64" s="23" t="s">
+      <c r="A64" s="19" t="s">
         <v>43</v>
       </c>
       <c r="B64" s="5" t="s">
@@ -1724,7 +1742,7 @@
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A65" s="23"/>
+      <c r="A65" s="19"/>
       <c r="B65" s="5" t="s">
         <v>0</v>
       </c>
@@ -1733,7 +1751,7 @@
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A66" s="23"/>
+      <c r="A66" s="19"/>
       <c r="B66" s="5" t="s">
         <v>2</v>
       </c>
@@ -1742,7 +1760,7 @@
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A67" s="23"/>
+      <c r="A67" s="19"/>
       <c r="B67" s="5" t="s">
         <v>9</v>
       </c>
@@ -1751,7 +1769,7 @@
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A68" s="23"/>
+      <c r="A68" s="19"/>
       <c r="B68" s="5" t="s">
         <v>3</v>
       </c>
@@ -1760,7 +1778,7 @@
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A69" s="23"/>
+      <c r="A69" s="19"/>
       <c r="B69" s="5" t="s">
         <v>1</v>
       </c>
@@ -1769,7 +1787,7 @@
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A70" s="23"/>
+      <c r="A70" s="19"/>
       <c r="B70" s="5" t="s">
         <v>85</v>
       </c>
@@ -1781,7 +1799,7 @@
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A71" s="23"/>
+      <c r="A71" s="19"/>
       <c r="B71" s="5" t="s">
         <v>21</v>
       </c>
@@ -1790,7 +1808,7 @@
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A72" s="23"/>
+      <c r="A72" s="19"/>
       <c r="B72" s="5" t="s">
         <v>15</v>
       </c>
@@ -1799,7 +1817,7 @@
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A73" s="23"/>
+      <c r="A73" s="19"/>
       <c r="B73" s="5" t="s">
         <v>81</v>
       </c>
@@ -1811,7 +1829,7 @@
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A74" s="23"/>
+      <c r="A74" s="19"/>
       <c r="B74" s="5" t="s">
         <v>82</v>
       </c>
@@ -1823,7 +1841,7 @@
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A75" s="23"/>
+      <c r="A75" s="19"/>
       <c r="B75" s="5" t="s">
         <v>64</v>
       </c>
@@ -1832,7 +1850,7 @@
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A76" s="23"/>
+      <c r="A76" s="19"/>
       <c r="B76" s="5" t="s">
         <v>65</v>
       </c>
@@ -1841,7 +1859,7 @@
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A77" s="23"/>
+      <c r="A77" s="19"/>
       <c r="B77" s="5" t="s">
         <v>66</v>
       </c>
@@ -1992,6 +2010,16 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A17:A28"/>
+    <mergeCell ref="A29:A34"/>
+    <mergeCell ref="A35:A37"/>
+    <mergeCell ref="A11:A16"/>
+    <mergeCell ref="A2:A10"/>
+    <mergeCell ref="A38:A41"/>
+    <mergeCell ref="A42:A45"/>
+    <mergeCell ref="A46:A48"/>
+    <mergeCell ref="A49:A52"/>
+    <mergeCell ref="A53:A56"/>
     <mergeCell ref="D42:D45"/>
     <mergeCell ref="A78:A87"/>
     <mergeCell ref="A88:A89"/>
@@ -1999,16 +2027,6 @@
     <mergeCell ref="A61:A63"/>
     <mergeCell ref="A64:A77"/>
     <mergeCell ref="A57:A60"/>
-    <mergeCell ref="A38:A41"/>
-    <mergeCell ref="A42:A45"/>
-    <mergeCell ref="A46:A48"/>
-    <mergeCell ref="A49:A52"/>
-    <mergeCell ref="A53:A56"/>
-    <mergeCell ref="A17:A28"/>
-    <mergeCell ref="A29:A34"/>
-    <mergeCell ref="A35:A37"/>
-    <mergeCell ref="A11:A16"/>
-    <mergeCell ref="A2:A10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2016,16 +2034,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H51"/>
+  <dimension ref="A1:H55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="226" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="212" workbookViewId="0">
+      <selection activeCell="F52" sqref="F52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="3"/>
-    <col min="2" max="2" width="14.33203125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="16" style="3" customWidth="1"/>
     <col min="3" max="3" width="10.83203125" style="13"/>
     <col min="4" max="16384" width="10.83203125" style="3"/>
   </cols>
@@ -2060,7 +2078,7 @@
       <c r="B2" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="23"/>
+      <c r="C2" s="19"/>
       <c r="D2" s="5" t="s">
         <v>109</v>
       </c>
@@ -2075,7 +2093,7 @@
       <c r="B3" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="C3" s="23"/>
+      <c r="C3" s="19"/>
       <c r="D3" s="5" t="s">
         <v>110</v>
       </c>
@@ -2090,7 +2108,7 @@
       <c r="B4" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="C4" s="23"/>
+      <c r="C4" s="19"/>
       <c r="D4" s="5" t="s">
         <v>117</v>
       </c>
@@ -2107,7 +2125,7 @@
       <c r="B5" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="C5" s="23"/>
+      <c r="C5" s="19"/>
       <c r="D5" s="5" t="s">
         <v>119</v>
       </c>
@@ -2124,7 +2142,7 @@
       <c r="B6" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="C6" s="23"/>
+      <c r="C6" s="19"/>
       <c r="D6" s="5" t="s">
         <v>120</v>
       </c>
@@ -2143,7 +2161,7 @@
       <c r="B7" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="C7" s="23"/>
+      <c r="C7" s="19"/>
       <c r="D7" s="5" t="s">
         <v>111</v>
       </c>
@@ -2162,7 +2180,7 @@
       <c r="B8" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="C8" s="23"/>
+      <c r="C8" s="19"/>
       <c r="D8" s="5" t="s">
         <v>112</v>
       </c>
@@ -2181,9 +2199,9 @@
       <c r="B9" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C9" s="23"/>
+      <c r="C9" s="19"/>
       <c r="D9" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>80</v>
@@ -2196,11 +2214,11 @@
         <v>92</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="C10" s="23"/>
+        <v>137</v>
+      </c>
+      <c r="C10" s="19"/>
       <c r="D10" s="7" t="s">
-        <v>137</v>
+        <v>172</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>80</v>
@@ -2217,7 +2235,7 @@
       <c r="B11" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="C11" s="23"/>
+      <c r="C11" s="19"/>
       <c r="D11" s="5" t="s">
         <v>113</v>
       </c>
@@ -2236,9 +2254,9 @@
       <c r="B12" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="23"/>
+      <c r="C12" s="19"/>
       <c r="D12" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>80</v>
@@ -2253,7 +2271,7 @@
       <c r="B13" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="C13" s="23"/>
+      <c r="C13" s="19"/>
       <c r="D13" s="5" t="s">
         <v>114</v>
       </c>
@@ -2272,7 +2290,7 @@
       <c r="B14" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="C14" s="23"/>
+      <c r="C14" s="19"/>
       <c r="D14" s="5" t="s">
         <v>119</v>
       </c>
@@ -2289,7 +2307,7 @@
       <c r="B15" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="C15" s="24" t="s">
+      <c r="C15" s="23" t="s">
         <v>133</v>
       </c>
       <c r="D15" s="7" t="s">
@@ -2310,7 +2328,7 @@
       <c r="B16" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="C16" s="24"/>
+      <c r="C16" s="23"/>
       <c r="D16" s="7" t="s">
         <v>111</v>
       </c>
@@ -2329,12 +2347,12 @@
       <c r="B17" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="C17" s="24"/>
+      <c r="C17" s="23"/>
       <c r="D17" s="14" t="s">
+        <v>143</v>
+      </c>
+      <c r="E17" s="14" t="s">
         <v>144</v>
-      </c>
-      <c r="E17" s="14" t="s">
-        <v>145</v>
       </c>
       <c r="F17" s="14" t="s">
         <v>38</v>
@@ -2348,7 +2366,7 @@
       <c r="B18" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="C18" s="24"/>
+      <c r="C18" s="23"/>
       <c r="D18" s="7" t="s">
         <v>135</v>
       </c>
@@ -2365,7 +2383,7 @@
       <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="23" t="s">
+      <c r="C19" s="19" t="s">
         <v>107</v>
       </c>
       <c r="D19" s="5" t="s">
@@ -2386,7 +2404,7 @@
       <c r="B20" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="23"/>
+      <c r="C20" s="19"/>
       <c r="D20" s="5" t="s">
         <v>101</v>
       </c>
@@ -2405,7 +2423,7 @@
       <c r="B21" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C21" s="23"/>
+      <c r="C21" s="19"/>
       <c r="D21" s="5" t="s">
         <v>102</v>
       </c>
@@ -2424,7 +2442,7 @@
       <c r="B22" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C22" s="23"/>
+      <c r="C22" s="19"/>
       <c r="D22" s="5" t="s">
         <v>103</v>
       </c>
@@ -2443,7 +2461,7 @@
       <c r="B23" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C23" s="23"/>
+      <c r="C23" s="19"/>
       <c r="D23" s="5" t="s">
         <v>104</v>
       </c>
@@ -2460,7 +2478,7 @@
       <c r="B24" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C24" s="23"/>
+      <c r="C24" s="19"/>
       <c r="D24" s="5" t="s">
         <v>105</v>
       </c>
@@ -2477,12 +2495,12 @@
       <c r="B25" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C25" s="23"/>
+      <c r="C25" s="19"/>
       <c r="D25" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F25" s="5" t="s">
         <v>80</v>
@@ -2496,9 +2514,9 @@
       <c r="B26" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C26" s="23"/>
+      <c r="C26" s="19"/>
       <c r="D26" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E26" s="14" t="s">
         <v>38</v>
@@ -2513,7 +2531,7 @@
       <c r="B27" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C27" s="23" t="s">
+      <c r="C27" s="19" t="s">
         <v>115</v>
       </c>
       <c r="D27" s="7" t="s">
@@ -2530,7 +2548,7 @@
       <c r="B28" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C28" s="23"/>
+      <c r="C28" s="19"/>
       <c r="D28" s="7" t="s">
         <v>102</v>
       </c>
@@ -2545,7 +2563,7 @@
       <c r="B29" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C29" s="23"/>
+      <c r="C29" s="19"/>
       <c r="D29" s="5" t="s">
         <v>103</v>
       </c>
@@ -2564,7 +2582,7 @@
       <c r="B30" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C30" s="23" t="s">
+      <c r="C30" s="19" t="s">
         <v>122</v>
       </c>
       <c r="D30" s="5" t="s">
@@ -2587,7 +2605,7 @@
       <c r="B31" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="C31" s="23"/>
+      <c r="C31" s="19"/>
       <c r="D31" s="5" t="s">
         <v>126</v>
       </c>
@@ -2606,7 +2624,7 @@
       <c r="B32" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="C32" s="23"/>
+      <c r="C32" s="19"/>
       <c r="D32" s="5" t="s">
         <v>127</v>
       </c>
@@ -2625,7 +2643,7 @@
       <c r="B33" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C33" s="23"/>
+      <c r="C33" s="19"/>
       <c r="D33" s="5" t="s">
         <v>128</v>
       </c>
@@ -2646,7 +2664,7 @@
       <c r="B34" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C34" s="23"/>
+      <c r="C34" s="19"/>
       <c r="D34" s="5" t="s">
         <v>132</v>
       </c>
@@ -2665,11 +2683,11 @@
         <v>92</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="C35" s="23"/>
+        <v>140</v>
+      </c>
+      <c r="C35" s="19"/>
       <c r="D35" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E35" s="7" t="s">
         <v>88</v>
@@ -2677,7 +2695,7 @@
       <c r="F35" s="7"/>
       <c r="G35" s="7"/>
       <c r="H35" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
@@ -2685,17 +2703,17 @@
         <v>92</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>167</v>
-      </c>
-      <c r="C36" s="23"/>
+        <v>166</v>
+      </c>
+      <c r="C36" s="19"/>
       <c r="D36" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E36" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="F36" s="7" t="s">
         <v>164</v>
-      </c>
-      <c r="F36" s="7" t="s">
-        <v>165</v>
       </c>
       <c r="G36" s="7" t="s">
         <v>88</v>
@@ -2706,14 +2724,14 @@
         <v>92</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>167</v>
-      </c>
-      <c r="C37" s="23"/>
+        <v>166</v>
+      </c>
+      <c r="C37" s="19"/>
       <c r="D37" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F37" s="7" t="s">
         <v>88</v>
@@ -2727,18 +2745,18 @@
       <c r="B38" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C38" s="23"/>
+      <c r="C38" s="19"/>
       <c r="D38" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E38" s="7" t="s">
         <v>89</v>
       </c>
       <c r="F38" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="G38" s="7" t="s">
         <v>169</v>
-      </c>
-      <c r="G38" s="7" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
@@ -2748,12 +2766,12 @@
       <c r="B39" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C39" s="23"/>
+      <c r="C39" s="19"/>
       <c r="D39" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="E39" s="7" t="s">
         <v>171</v>
-      </c>
-      <c r="E39" s="7" t="s">
-        <v>172</v>
       </c>
       <c r="F39" s="7"/>
       <c r="G39" s="7"/>
@@ -2765,17 +2783,17 @@
       <c r="B40" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C40" s="23"/>
-      <c r="D40" s="15" t="s">
+      <c r="C40" s="19"/>
+      <c r="D40" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="E40" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="F40" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="E40" s="15" t="s">
-        <v>89</v>
-      </c>
-      <c r="F40" s="15" t="s">
-        <v>152</v>
-      </c>
-      <c r="G40" s="15"/>
+      <c r="G40" s="7"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="5" t="s">
@@ -2784,17 +2802,17 @@
       <c r="B41" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C41" s="23"/>
-      <c r="D41" s="15" t="s">
-        <v>156</v>
-      </c>
-      <c r="E41" s="15" t="s">
+      <c r="C41" s="19"/>
+      <c r="D41" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="E41" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="F41" s="15" t="s">
-        <v>152</v>
-      </c>
-      <c r="G41" s="15"/>
+      <c r="F41" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="G41" s="7"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="5" t="s">
@@ -2803,15 +2821,15 @@
       <c r="B42" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C42" s="23"/>
+      <c r="C42" s="19"/>
       <c r="D42" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E42" s="7" t="s">
         <v>89</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G42" s="7"/>
     </row>
@@ -2822,15 +2840,15 @@
       <c r="B43" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C43" s="23"/>
+      <c r="C43" s="19"/>
       <c r="D43" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E43" s="7" t="s">
         <v>89</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G43" s="7"/>
     </row>
@@ -2841,7 +2859,7 @@
       <c r="B44" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C44" s="23"/>
+      <c r="C44" s="19"/>
       <c r="D44" s="7" t="s">
         <v>135</v>
       </c>
@@ -2856,16 +2874,16 @@
         <v>92</v>
       </c>
       <c r="B45" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="C45" s="19" t="s">
         <v>141</v>
-      </c>
-      <c r="C45" s="23" t="s">
-        <v>142</v>
       </c>
       <c r="D45" s="7" t="s">
         <v>105</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F45" s="7" t="s">
         <v>0</v>
@@ -2881,7 +2899,7 @@
       <c r="B46" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="C46" s="23"/>
+      <c r="C46" s="19"/>
       <c r="D46" s="7" t="s">
         <v>113</v>
       </c>
@@ -2900,9 +2918,9 @@
       <c r="B47" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="C47" s="23"/>
+      <c r="C47" s="19"/>
       <c r="D47" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E47" s="7" t="s">
         <v>0</v>
@@ -2919,12 +2937,12 @@
       <c r="B48" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="C48" s="23"/>
+      <c r="C48" s="19"/>
       <c r="D48" s="7" t="s">
         <v>111</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F48" s="7" t="s">
         <v>0</v>
@@ -2940,11 +2958,11 @@
       <c r="B49" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C49" s="23" t="s">
-        <v>147</v>
+      <c r="C49" s="19" t="s">
+        <v>146</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E49" s="5"/>
       <c r="F49" s="5"/>
@@ -2957,9 +2975,9 @@
       <c r="B50" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C50" s="23"/>
+      <c r="C50" s="19"/>
       <c r="D50" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E50" s="5"/>
       <c r="F50" s="5"/>
@@ -2970,18 +2988,93 @@
         <v>91</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="C51" s="23"/>
+        <v>145</v>
+      </c>
+      <c r="C51" s="19"/>
       <c r="D51" s="7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E51" s="7"/>
       <c r="F51" s="7"/>
       <c r="G51" s="7"/>
     </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A52" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="C52" s="16" t="s">
+        <v>173</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="E52" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F52" s="5"/>
+      <c r="G52" s="5"/>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A53" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="C53" s="17"/>
+      <c r="D53" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="E53" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F53" s="5"/>
+      <c r="G53" s="5"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A54" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="C54" s="17"/>
+      <c r="D54" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="E54" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="F54" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="G54" s="5" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A55" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="C55" s="18"/>
+      <c r="D55" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="E55" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="F55" s="5"/>
+      <c r="G55" s="5"/>
+    </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
+    <mergeCell ref="C52:C55"/>
     <mergeCell ref="C49:C51"/>
     <mergeCell ref="C2:C14"/>
     <mergeCell ref="C45:C48"/>

</xml_diff>